<commit_message>
Sentiment Scores as floats
</commit_message>
<xml_diff>
--- a/Annotations - Simon.xlsx
+++ b/Annotations - Simon.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SimonU\CognitiveSystems\Advanced Natural Language Processing\Course Project\ANLP_Final_Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tabellenblatt1" sheetId="1" r:id="rId3"/>
+    <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
   <si>
     <t>Sentiment</t>
   </si>
@@ -46,9 +54,6 @@
     <t>Article 20</t>
   </si>
   <si>
-    <t>neutral</t>
-  </si>
-  <si>
     <t>Inquiries of Brexit</t>
   </si>
   <si>
@@ -64,9 +69,6 @@
     <t>Article 21</t>
   </si>
   <si>
-    <t>rather negative</t>
-  </si>
-  <si>
     <t>rising consumer prices/Currency value drop</t>
   </si>
   <si>
@@ -133,9 +135,6 @@
     <t>Article 25</t>
   </si>
   <si>
-    <t>negative</t>
-  </si>
-  <si>
     <t>kind of brexit deal</t>
   </si>
   <si>
@@ -163,27 +162,18 @@
     <t>Article 29</t>
   </si>
   <si>
-    <t>rather positive</t>
-  </si>
-  <si>
     <t>Article 30</t>
   </si>
   <si>
     <t>Article 31</t>
   </si>
   <si>
-    <t>neutral to negative</t>
-  </si>
-  <si>
     <t>Article 32</t>
   </si>
   <si>
     <t>Article 33</t>
   </si>
   <si>
-    <t>positive</t>
-  </si>
-  <si>
     <t>Article 34</t>
   </si>
   <si>
@@ -200,9 +190,6 @@
   </si>
   <si>
     <t>Article 39</t>
-  </si>
-  <si>
-    <t>rather neutral</t>
   </si>
   <si>
     <t>Telegraph</t>
@@ -253,79 +240,350 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="27.14"/>
-    <col customWidth="1" min="4" max="5" width="27.71"/>
-    <col customWidth="1" min="6" max="6" width="46.0"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -357,29 +615,29 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
@@ -388,77 +646,77 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="H4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -468,24 +726,24 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -494,27 +752,27 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-0.8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="G8" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -522,12 +780,12 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -540,12 +798,12 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -558,12 +816,12 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -576,12 +834,12 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.3</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -594,12 +852,12 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.3</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -612,12 +870,12 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-0.1</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -630,12 +888,12 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -648,12 +906,12 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.8</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -666,12 +924,12 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>51</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -684,12 +942,12 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -702,12 +960,12 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>53</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -720,12 +978,12 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-0.8</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -738,12 +996,12 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -756,12 +1014,12 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -774,7 +1032,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -787,9 +1045,9 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -802,18 +1060,18 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>17</v>
+      <c r="B25" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -824,27 +1082,27 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -852,18 +1110,18 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="B27" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -874,18 +1132,18 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -896,18 +1154,18 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="B29" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -918,12 +1176,12 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -936,15 +1194,15 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
+      </c>
+      <c r="B31" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -956,12 +1214,12 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>17</v>
+        <v>44</v>
+      </c>
+      <c r="B32" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -974,12 +1232,12 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -992,12 +1250,12 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1010,12 +1268,12 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
+      </c>
+      <c r="B35" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1028,12 +1286,12 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>17</v>
+        <v>48</v>
+      </c>
+      <c r="B36" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1046,12 +1304,12 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1064,12 +1322,12 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1082,12 +1340,12 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>11</v>
+        <v>51</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1100,12 +1358,12 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1118,12 +1376,12 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>17</v>
+        <v>53</v>
+      </c>
+      <c r="B41" s="2">
+        <v>-0.3</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1136,12 +1394,12 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1154,23 +1412,23 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>55</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>17</v>
+        <v>56</v>
+      </c>
+      <c r="B44" s="2">
+        <v>-0.3</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>